<commit_message>
update para recibir flotantes
update para recibir flotantes
</commit_message>
<xml_diff>
--- a/Analisis/inventario promedio.xlsx
+++ b/Analisis/inventario promedio.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB08082-77C6-432F-8EAE-C0FEE8D0E40A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8FBDCA-02AA-4643-9785-F4219F49B9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B267885A-95E7-AA43-BFF7-CD54C9E1CB7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -514,15 +517,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B97FD8-331F-A24E-8148-6D213DD2ECDD}">
   <dimension ref="B1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.75" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.375" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.625" style="1" customWidth="1"/>
@@ -621,7 +625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>